<commit_message>
bug fixes gedaan en begin admin page gemaakt
</commit_message>
<xml_diff>
--- a/Documenten/Logboek.xlsx
+++ b/Documenten/Logboek.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="48">
   <si>
     <t>Datum</t>
   </si>
@@ -165,6 +165,9 @@
   </si>
   <si>
     <t>Login en user_page samengehangen</t>
+  </si>
+  <si>
+    <t>Login en check in worden op 1 gezet in databank en worden juist getoont op de user page</t>
   </si>
 </sst>
 </file>
@@ -549,7 +552,7 @@
   <dimension ref="A1:P47"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D30" sqref="D30"/>
+      <selection activeCell="A32" sqref="A32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1019,7 +1022,18 @@
       </c>
     </row>
     <row r="31" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A31" s="1"/>
+      <c r="A31" s="1">
+        <v>42825</v>
+      </c>
+      <c r="B31" t="s">
+        <v>47</v>
+      </c>
+      <c r="C31">
+        <v>2.5</v>
+      </c>
+      <c r="D31" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="32" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A32" s="1"/>

</xml_diff>

<commit_message>
logboek en verslag servers phpmyadmin
</commit_message>
<xml_diff>
--- a/Documenten/Logboek.xlsx
+++ b/Documenten/Logboek.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="126">
   <si>
     <t>Datum</t>
   </si>
@@ -168,22 +168,252 @@
   </si>
   <si>
     <t>Login en check in worden op 1 gezet in databank en worden juist getoont op de user page</t>
+  </si>
+  <si>
+    <t>bug fixes gedaan en begin admin page gemaakt</t>
+  </si>
+  <si>
+    <t>verder gewerkt aan admin page</t>
+  </si>
+  <si>
+    <t>info page aangemaakt</t>
+  </si>
+  <si>
+    <t>start date toegevoegd aan database en start date bij info pagina</t>
+  </si>
+  <si>
+    <t>info page afgewerkt</t>
+  </si>
+  <si>
+    <t>testgebruikers toegevoegd</t>
+  </si>
+  <si>
+    <t>script gemaakt voor users af te drukken op scherm</t>
+  </si>
+  <si>
+    <t>databank aangepast en e-r diagramma aangepast</t>
+  </si>
+  <si>
+    <t>Check in werkt</t>
+  </si>
+  <si>
+    <t>Check in en out werkt</t>
+  </si>
+  <si>
+    <t>veranderingen verder doorgevoerd in andere pagina's</t>
+  </si>
+  <si>
+    <t>database aangepast voor check in en out en logout wordt geregistreerd in databank</t>
+  </si>
+  <si>
+    <t>de "in building" query naar functions.php verplaatst</t>
+  </si>
+  <si>
+    <t>kleine bug bij het nakijken in building</t>
+  </si>
+  <si>
+    <t>tests uitgevoerd op databank</t>
+  </si>
+  <si>
+    <t>bug bij de lijst van de users</t>
+  </si>
+  <si>
+    <t>tooltip bijgevoegd overal waar er "national insurance number" staat</t>
+  </si>
+  <si>
+    <t>de figuurtjes voor "ingelogd" en "in building" in de website gezet</t>
+  </si>
+  <si>
+    <t>colleague info page klaar</t>
+  </si>
+  <si>
+    <t>bug op colleague info page gefixt</t>
+  </si>
+  <si>
+    <t>info word automatisch ingevuld op settings page</t>
+  </si>
+  <si>
+    <t>check in out chart begonnen</t>
+  </si>
+  <si>
+    <t>Settings werken</t>
+  </si>
+  <si>
+    <t>begonnen aan user manage voor de admin</t>
+  </si>
+  <si>
+    <t>begonnen aan user add voor de admin</t>
+  </si>
+  <si>
+    <t>user bijvoegen werkt aleen de rechten worden niet geregistreerd</t>
+  </si>
+  <si>
+    <t>bug bij het bijvoegen van een user gefixt</t>
+  </si>
+  <si>
+    <t>bij de userpage word de foto getoont</t>
+  </si>
+  <si>
+    <t>messages komen in de databank vanaf colleague page</t>
+  </si>
+  <si>
+    <t>men kan berichten sturen vanaf messages page</t>
+  </si>
+  <si>
+    <t>message page is in orde</t>
+  </si>
+  <si>
+    <t>nieuwe testdata en de berichten worden weergegeven op een andere pagina</t>
+  </si>
+  <si>
+    <t>message page verder uitgewerkt</t>
+  </si>
+  <si>
+    <t>begonnen aan search functie</t>
+  </si>
+  <si>
+    <t>search werk bij de messages</t>
+  </si>
+  <si>
+    <t>ervoor gezorgd dat men geen berichten kan openen die men niet mag openen</t>
+  </si>
+  <si>
+    <t>opmaak bij user add page een beetje aangepast</t>
+  </si>
+  <si>
+    <t>telefoonnummer werd getoont zonder de 0 vooraan, opgelost</t>
+  </si>
+  <si>
+    <t>user bewerken is in orde</t>
+  </si>
+  <si>
+    <t>men kan de berichten nog niet openen en ook niet zoeken</t>
+  </si>
+  <si>
+    <t>users verwijderen is in orde</t>
+  </si>
+  <si>
+    <t>bug fixes</t>
+  </si>
+  <si>
+    <t>nog een paar bugs gevonden en opgelost</t>
+  </si>
+  <si>
+    <t>check in en out grafiek verder aan gewerkt</t>
+  </si>
+  <si>
+    <t>er komt een popup bij de message als men een bericht krijgt en de ongelezen berichten hebben een kleurtje</t>
+  </si>
+  <si>
+    <t>bij het antwoorden op een bericht word bij topic automatisch "RE:" toegevoegd</t>
+  </si>
+  <si>
+    <t>bug bij het zoeken naar berichten opgelost</t>
+  </si>
+  <si>
+    <t>ckeck_in_out_page_colleague.php en messages_page_colleague.php aangemaakt, alle pagina's zijn gemaakt</t>
+  </si>
+  <si>
+    <t>bugs opgelost</t>
+  </si>
+  <si>
+    <t>mobiele optimalisatie in orde</t>
+  </si>
+  <si>
+    <t>bug waneer men als admin een bericht van iemand anders bekijkt dit op gelezen staat, opgelost</t>
+  </si>
+  <si>
+    <t>men kan files toevoegen aan een bericht</t>
+  </si>
+  <si>
+    <t>men kan nu maar 1 keer per dag in en uitchecken, nodig voor de grafiek</t>
+  </si>
+  <si>
+    <t>bug bij de user, opgelost door de user terug in te loggen waneer men refresht</t>
+  </si>
+  <si>
+    <t>user zijn session word elke 2 seconden opniem ingevuld</t>
+  </si>
+  <si>
+    <t>de auto refresh werkt terug bij de check in</t>
+  </si>
+  <si>
+    <t>opmaak van de admin pages bijgewerkt</t>
+  </si>
+  <si>
+    <t>file icoontje bij messages gezet</t>
+  </si>
+  <si>
+    <t>search functie verbeterd</t>
+  </si>
+  <si>
+    <t>kleine bugfix</t>
+  </si>
+  <si>
+    <t>waneer er geen ongelezen messages zijn word de badge niet getoont</t>
+  </si>
+  <si>
+    <t>nog kleine bugs opgelost</t>
+  </si>
+  <si>
+    <t>bugfixes</t>
+  </si>
+  <si>
+    <t>waneer er bij admin_add een veld niet word ingevuld krijgt men een waarschuwing</t>
+  </si>
+  <si>
+    <t>overlimit button aangemaakt</t>
+  </si>
+  <si>
+    <t>overlimit button bugs poberen oplossen</t>
+  </si>
+  <si>
+    <t>bij user manage page een link gezet naar de user zijn acount</t>
+  </si>
+  <si>
+    <t>overlimit button verder bewerkt</t>
+  </si>
+  <si>
+    <t>op de virtuele server 3 servers aangemaakt voor de failover cluster voor de webserver</t>
+  </si>
+  <si>
+    <t>een domaincontroller en een domain aangemaakt op een nieuwe virtuele server</t>
+  </si>
+  <si>
+    <t>ook een storage server aangemakt voor de fileserver</t>
+  </si>
+  <si>
+    <t>al de servers in het domain gezet</t>
+  </si>
+  <si>
+    <t>op de webservers apache gëinstaleerd en de source map voor de .php files op de fileserver gezet</t>
+  </si>
+  <si>
+    <t>op de failover cluster ook een fileserver gezet die de storage van de storageserver gebruikt</t>
+  </si>
+  <si>
+    <t>geprobeerd op de databank ook op de fileshare te zetten maar dit is niet gelukt</t>
+  </si>
+  <si>
+    <t>een apparte server aangemaakt voor de databank op te hosten</t>
+  </si>
+  <si>
+    <t>op de databank server de firewal instellingen aangepast en een databank op geinstaleerd en de sql file geinporteerd</t>
+  </si>
+  <si>
+    <t>alle files voor de website overgezet op de fileserver zodat de webservers ze kunnen gebruiken</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="165" formatCode="d/mm/yyyy;@"/>
+  </numFmts>
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="18"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -210,17 +440,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standaard" xfId="0" builtinId="0"/>
@@ -239,8 +470,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Tabel3" displayName="Tabel3" ref="A1:E53" totalsRowShown="0">
-  <autoFilter ref="A1:E53"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Tabel3" displayName="Tabel3" ref="A1:E130" totalsRowShown="0">
+  <autoFilter ref="A1:E130"/>
   <tableColumns count="5">
     <tableColumn id="1" name="Datum"/>
     <tableColumn id="2" name="Wat gedaan?"/>
@@ -549,10 +780,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P47"/>
+  <dimension ref="A1:P122"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A32" sqref="A32"/>
+      <selection activeCell="C2" sqref="C2:C114"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -826,20 +1057,20 @@
         <v>6</v>
       </c>
     </row>
-    <row r="18" spans="1:16" s="5" customFormat="1" ht="60" x14ac:dyDescent="0.25">
-      <c r="A18" s="4">
+    <row r="18" spans="1:16" s="4" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+      <c r="A18" s="3">
         <v>42810</v>
       </c>
-      <c r="B18" s="5" t="s">
+      <c r="B18" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="C18" s="5">
+      <c r="C18" s="4">
         <v>4</v>
       </c>
-      <c r="D18" s="5" t="s">
+      <c r="D18" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="E18" s="5" t="s">
+      <c r="E18" s="4" t="s">
         <v>39</v>
       </c>
     </row>
@@ -985,7 +1216,7 @@
       <c r="D28" t="s">
         <v>9</v>
       </c>
-      <c r="E28" s="5" t="s">
+      <c r="E28" s="4" t="s">
         <v>44</v>
       </c>
       <c r="P28" t="e">
@@ -998,24 +1229,25 @@
         <v>42823</v>
       </c>
       <c r="B29" t="s">
-        <v>45</v>
+        <v>116</v>
       </c>
       <c r="C29">
         <v>2</v>
       </c>
       <c r="D29" t="s">
-        <v>5</v>
-      </c>
+        <v>9</v>
+      </c>
+      <c r="E29" s="4"/>
     </row>
     <row r="30" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
-        <v>42824</v>
+        <v>42823</v>
       </c>
       <c r="B30" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C30">
-        <v>1.5</v>
+        <v>2</v>
       </c>
       <c r="D30" t="s">
         <v>5</v>
@@ -1023,66 +1255,1144 @@
     </row>
     <row r="31" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
+        <v>42824</v>
+      </c>
+      <c r="B31" t="s">
+        <v>46</v>
+      </c>
+      <c r="C31">
+        <v>1.5</v>
+      </c>
+      <c r="D31" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="32" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A32" s="1">
         <v>42825</v>
       </c>
-      <c r="B31" t="s">
+      <c r="B32" t="s">
         <v>47</v>
       </c>
-      <c r="C31">
+      <c r="C32">
         <v>2.5</v>
       </c>
-      <c r="D31" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="32" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A32" s="1"/>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33" s="1"/>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A34" s="1"/>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A35" s="1"/>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A36" s="1"/>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A37" s="1"/>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A38" s="1"/>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A39" s="1"/>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A40" s="1"/>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A41" s="1"/>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A42" s="1"/>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A43" s="1"/>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A44" s="1"/>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A45" s="1"/>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A46" s="1"/>
-    </row>
-    <row r="47" spans="1:3" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B47" s="3"/>
-      <c r="C47" s="3"/>
+      <c r="D32" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" s="1">
+        <v>42826</v>
+      </c>
+      <c r="B33" t="s">
+        <v>48</v>
+      </c>
+      <c r="C33">
+        <v>3</v>
+      </c>
+      <c r="D33" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" s="1">
+        <v>42831</v>
+      </c>
+      <c r="B34" t="s">
+        <v>49</v>
+      </c>
+      <c r="C34">
+        <v>0.5</v>
+      </c>
+      <c r="D34" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" s="1">
+        <v>42831</v>
+      </c>
+      <c r="B35" t="s">
+        <v>50</v>
+      </c>
+      <c r="C35">
+        <v>1</v>
+      </c>
+      <c r="D35" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" s="1">
+        <v>42831</v>
+      </c>
+      <c r="B36" t="s">
+        <v>51</v>
+      </c>
+      <c r="C36">
+        <v>0.5</v>
+      </c>
+      <c r="D36" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" s="1">
+        <v>42831</v>
+      </c>
+      <c r="B37" t="s">
+        <v>52</v>
+      </c>
+      <c r="C37">
+        <v>1</v>
+      </c>
+      <c r="D37" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" s="1">
+        <v>42831</v>
+      </c>
+      <c r="B38" t="s">
+        <v>53</v>
+      </c>
+      <c r="C38">
+        <v>0.1</v>
+      </c>
+      <c r="D38" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39" s="1">
+        <v>42831</v>
+      </c>
+      <c r="B39" t="s">
+        <v>54</v>
+      </c>
+      <c r="C39">
+        <v>1</v>
+      </c>
+      <c r="D39" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40" s="1">
+        <v>42832</v>
+      </c>
+      <c r="B40" t="s">
+        <v>55</v>
+      </c>
+      <c r="C40">
+        <v>0.75</v>
+      </c>
+      <c r="D40" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41" s="1">
+        <v>42832</v>
+      </c>
+      <c r="B41" t="s">
+        <v>56</v>
+      </c>
+      <c r="C41">
+        <v>1</v>
+      </c>
+      <c r="D41" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42" s="1">
+        <v>42832</v>
+      </c>
+      <c r="B42" t="s">
+        <v>57</v>
+      </c>
+      <c r="C42">
+        <v>1.5</v>
+      </c>
+      <c r="D42" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A43" s="1">
+        <v>42832</v>
+      </c>
+      <c r="B43" t="s">
+        <v>58</v>
+      </c>
+      <c r="C43">
+        <v>0.75</v>
+      </c>
+      <c r="D43" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A44" s="1">
+        <v>42832</v>
+      </c>
+      <c r="B44" t="s">
+        <v>59</v>
+      </c>
+      <c r="C44">
+        <v>0.75</v>
+      </c>
+      <c r="D44" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A45" s="1">
+        <v>42832</v>
+      </c>
+      <c r="B45" t="s">
+        <v>60</v>
+      </c>
+      <c r="C45">
+        <v>0.2</v>
+      </c>
+      <c r="D45" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A46" s="1">
+        <v>42832</v>
+      </c>
+      <c r="B46" t="s">
+        <v>61</v>
+      </c>
+      <c r="C46">
+        <v>0.2</v>
+      </c>
+      <c r="D46" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A47" s="1">
+        <v>42832</v>
+      </c>
+      <c r="B47" t="s">
+        <v>62</v>
+      </c>
+      <c r="C47">
+        <v>1</v>
+      </c>
+      <c r="D47" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A48" s="1">
+        <v>42833</v>
+      </c>
+      <c r="B48" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="C48" s="5">
+        <v>0.4</v>
+      </c>
+      <c r="D48" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A49" s="6">
+        <v>42833</v>
+      </c>
+      <c r="B49" t="s">
+        <v>64</v>
+      </c>
+      <c r="C49">
+        <v>0.75</v>
+      </c>
+      <c r="D49" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A50" s="6">
+        <v>42833</v>
+      </c>
+      <c r="B50" t="s">
+        <v>65</v>
+      </c>
+      <c r="C50">
+        <v>1.5</v>
+      </c>
+      <c r="D50" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A51" s="6">
+        <v>42833</v>
+      </c>
+      <c r="B51" t="s">
+        <v>66</v>
+      </c>
+      <c r="C51">
+        <v>1</v>
+      </c>
+      <c r="D51" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A52" s="6">
+        <v>42833</v>
+      </c>
+      <c r="B52" t="s">
+        <v>67</v>
+      </c>
+      <c r="C52">
+        <v>0.2</v>
+      </c>
+      <c r="D52" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A53" s="6">
+        <v>42833</v>
+      </c>
+      <c r="B53" t="s">
+        <v>68</v>
+      </c>
+      <c r="C53">
+        <v>1.2</v>
+      </c>
+      <c r="D53" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A54" s="6">
+        <v>42836</v>
+      </c>
+      <c r="B54" t="s">
+        <v>69</v>
+      </c>
+      <c r="C54">
+        <v>2</v>
+      </c>
+      <c r="D54" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A55" s="6">
+        <v>42839</v>
+      </c>
+      <c r="B55" t="s">
+        <v>70</v>
+      </c>
+      <c r="C55">
+        <v>1.5</v>
+      </c>
+      <c r="D55" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A56" s="6">
+        <v>42844</v>
+      </c>
+      <c r="B56" t="s">
+        <v>117</v>
+      </c>
+      <c r="C56">
+        <v>2</v>
+      </c>
+      <c r="D56" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A57" s="6">
+        <v>42844</v>
+      </c>
+      <c r="B57" t="s">
+        <v>118</v>
+      </c>
+      <c r="C57">
+        <v>1</v>
+      </c>
+      <c r="D57" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A58" s="6">
+        <v>42844</v>
+      </c>
+      <c r="B58" t="s">
+        <v>119</v>
+      </c>
+      <c r="C58">
+        <v>0.75</v>
+      </c>
+      <c r="D58" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A59" s="6">
+        <v>42844</v>
+      </c>
+      <c r="B59" t="s">
+        <v>71</v>
+      </c>
+      <c r="C59">
+        <v>1</v>
+      </c>
+      <c r="D59" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A60" s="6">
+        <v>42844</v>
+      </c>
+      <c r="B60" t="s">
+        <v>72</v>
+      </c>
+      <c r="C60">
+        <v>0.5</v>
+      </c>
+      <c r="D60" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A61" s="6">
+        <v>42844</v>
+      </c>
+      <c r="B61" t="s">
+        <v>73</v>
+      </c>
+      <c r="C61">
+        <v>1</v>
+      </c>
+      <c r="D61" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A62" s="6">
+        <v>42844</v>
+      </c>
+      <c r="B62" t="s">
+        <v>74</v>
+      </c>
+      <c r="C62">
+        <v>0.5</v>
+      </c>
+      <c r="D62" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A63" s="6">
+        <v>42844</v>
+      </c>
+      <c r="B63" t="s">
+        <v>75</v>
+      </c>
+      <c r="C63">
+        <v>0.5</v>
+      </c>
+      <c r="D63" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A64" s="6">
+        <v>42844</v>
+      </c>
+      <c r="B64" t="s">
+        <v>76</v>
+      </c>
+      <c r="C64">
+        <v>0.75</v>
+      </c>
+      <c r="D64" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A65" s="6">
+        <v>42844</v>
+      </c>
+      <c r="B65" t="s">
+        <v>77</v>
+      </c>
+      <c r="C65">
+        <v>0.75</v>
+      </c>
+      <c r="D65" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A66" s="6">
+        <v>42845</v>
+      </c>
+      <c r="B66" t="s">
+        <v>78</v>
+      </c>
+      <c r="C66">
+        <v>0.5</v>
+      </c>
+      <c r="D66" t="s">
+        <v>6</v>
+      </c>
+      <c r="E66" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A67" s="6">
+        <v>42845</v>
+      </c>
+      <c r="B67" t="s">
+        <v>79</v>
+      </c>
+      <c r="C67">
+        <v>0.75</v>
+      </c>
+      <c r="D67" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A68" s="6">
+        <v>42845</v>
+      </c>
+      <c r="B68" t="s">
+        <v>80</v>
+      </c>
+      <c r="C68">
+        <v>1</v>
+      </c>
+      <c r="D68" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A69" s="6">
+        <v>42845</v>
+      </c>
+      <c r="B69" t="s">
+        <v>81</v>
+      </c>
+      <c r="C69">
+        <v>0.5</v>
+      </c>
+      <c r="D69" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A70" s="6">
+        <v>42848</v>
+      </c>
+      <c r="B70" t="s">
+        <v>82</v>
+      </c>
+      <c r="C70">
+        <v>2</v>
+      </c>
+      <c r="D70" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A71" s="6">
+        <v>42848</v>
+      </c>
+      <c r="B71" t="s">
+        <v>83</v>
+      </c>
+      <c r="C71">
+        <v>0.5</v>
+      </c>
+      <c r="D71" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A72" s="6">
+        <v>42848</v>
+      </c>
+      <c r="B72" t="s">
+        <v>84</v>
+      </c>
+      <c r="C72">
+        <v>0.5</v>
+      </c>
+      <c r="D72" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A73" s="6">
+        <v>42848</v>
+      </c>
+      <c r="B73" t="s">
+        <v>85</v>
+      </c>
+      <c r="C73">
+        <v>0.75</v>
+      </c>
+      <c r="D73" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A74" s="6">
+        <v>42848</v>
+      </c>
+      <c r="B74" t="s">
+        <v>86</v>
+      </c>
+      <c r="C74">
+        <v>1.5</v>
+      </c>
+      <c r="D74" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A75" s="6">
+        <v>42848</v>
+      </c>
+      <c r="B75" t="s">
+        <v>88</v>
+      </c>
+      <c r="C75">
+        <v>0.75</v>
+      </c>
+      <c r="D75" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A76" s="6">
+        <v>42848</v>
+      </c>
+      <c r="B76" t="s">
+        <v>89</v>
+      </c>
+      <c r="C76">
+        <v>1</v>
+      </c>
+      <c r="D76" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A77" s="6">
+        <v>42851</v>
+      </c>
+      <c r="B77" t="s">
+        <v>121</v>
+      </c>
+      <c r="C77">
+        <v>1.75</v>
+      </c>
+      <c r="D77" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A78" s="6">
+        <v>42851</v>
+      </c>
+      <c r="B78" t="s">
+        <v>120</v>
+      </c>
+      <c r="C78">
+        <v>2</v>
+      </c>
+      <c r="D78" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A79" s="6">
+        <v>42851</v>
+      </c>
+      <c r="B79" t="s">
+        <v>122</v>
+      </c>
+      <c r="C79">
+        <v>1.5</v>
+      </c>
+      <c r="D79" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A80" s="6">
+        <v>42851</v>
+      </c>
+      <c r="B80" t="s">
+        <v>90</v>
+      </c>
+      <c r="C80">
+        <v>0.75</v>
+      </c>
+      <c r="D80" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A81" s="6">
+        <v>42851</v>
+      </c>
+      <c r="B81" t="s">
+        <v>91</v>
+      </c>
+      <c r="C81">
+        <v>1.5</v>
+      </c>
+      <c r="D81" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A82" s="6">
+        <v>42851</v>
+      </c>
+      <c r="B82" t="s">
+        <v>92</v>
+      </c>
+      <c r="C82">
+        <v>1.75</v>
+      </c>
+      <c r="D82" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A83" s="6">
+        <v>42851</v>
+      </c>
+      <c r="B83" t="s">
+        <v>93</v>
+      </c>
+      <c r="C83">
+        <v>0.5</v>
+      </c>
+      <c r="D83" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A84" s="6">
+        <v>42851</v>
+      </c>
+      <c r="B84" t="s">
+        <v>94</v>
+      </c>
+      <c r="C84">
+        <v>0.5</v>
+      </c>
+      <c r="D84" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A85" s="6">
+        <v>42851</v>
+      </c>
+      <c r="B85" t="s">
+        <v>95</v>
+      </c>
+      <c r="C85">
+        <v>0.75</v>
+      </c>
+      <c r="D85" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A86" s="6">
+        <v>42851</v>
+      </c>
+      <c r="B86" t="s">
+        <v>96</v>
+      </c>
+      <c r="C86">
+        <v>0.5</v>
+      </c>
+      <c r="D86" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A87" s="6">
+        <v>42851</v>
+      </c>
+      <c r="B87" t="s">
+        <v>97</v>
+      </c>
+      <c r="C87">
+        <v>0.75</v>
+      </c>
+      <c r="D87" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A88" s="6">
+        <v>42852</v>
+      </c>
+      <c r="B88" t="s">
+        <v>98</v>
+      </c>
+      <c r="C88">
+        <v>0.5</v>
+      </c>
+      <c r="D88" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A89" s="6">
+        <v>42852</v>
+      </c>
+      <c r="B89" t="s">
+        <v>99</v>
+      </c>
+      <c r="C89">
+        <v>1.5</v>
+      </c>
+      <c r="D89" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A90" s="6">
+        <v>42852</v>
+      </c>
+      <c r="B90" t="s">
+        <v>100</v>
+      </c>
+      <c r="C90">
+        <v>1</v>
+      </c>
+      <c r="D90" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A91" s="6">
+        <v>42852</v>
+      </c>
+      <c r="B91" t="s">
+        <v>101</v>
+      </c>
+      <c r="C91">
+        <v>0.5</v>
+      </c>
+      <c r="D91" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A92" s="6">
+        <v>42852</v>
+      </c>
+      <c r="B92" t="s">
+        <v>102</v>
+      </c>
+      <c r="C92">
+        <v>0.2</v>
+      </c>
+      <c r="D92" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A93" s="6">
+        <v>42857</v>
+      </c>
+      <c r="B93" t="s">
+        <v>103</v>
+      </c>
+      <c r="C93">
+        <v>0.5</v>
+      </c>
+      <c r="D93" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A94" s="6">
+        <v>42857</v>
+      </c>
+      <c r="B94" t="s">
+        <v>104</v>
+      </c>
+      <c r="C94">
+        <v>0.75</v>
+      </c>
+      <c r="D94" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A95" s="6">
+        <v>42857</v>
+      </c>
+      <c r="B95" t="s">
+        <v>105</v>
+      </c>
+      <c r="C95">
+        <v>0.3</v>
+      </c>
+      <c r="D95" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A96" s="6">
+        <v>42857</v>
+      </c>
+      <c r="B96" t="s">
+        <v>106</v>
+      </c>
+      <c r="C96">
+        <v>0.4</v>
+      </c>
+      <c r="D96" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A97" s="6">
+        <v>42857</v>
+      </c>
+      <c r="B97" t="s">
+        <v>107</v>
+      </c>
+      <c r="C97">
+        <v>0.2</v>
+      </c>
+      <c r="D97" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A98" s="6">
+        <v>42857</v>
+      </c>
+      <c r="B98" t="s">
+        <v>108</v>
+      </c>
+      <c r="C98">
+        <v>0.4</v>
+      </c>
+      <c r="D98" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A99" s="6">
+        <v>42857</v>
+      </c>
+      <c r="B99" t="s">
+        <v>109</v>
+      </c>
+      <c r="C99">
+        <v>0.3</v>
+      </c>
+      <c r="D99" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A100" s="6">
+        <v>42857</v>
+      </c>
+      <c r="B100" t="s">
+        <v>110</v>
+      </c>
+      <c r="C100">
+        <v>0.4</v>
+      </c>
+      <c r="D100" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A101" s="6">
+        <v>42858</v>
+      </c>
+      <c r="B101" t="s">
+        <v>111</v>
+      </c>
+      <c r="C101">
+        <v>0.3</v>
+      </c>
+      <c r="D101" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A102" s="6">
+        <v>42858</v>
+      </c>
+      <c r="B102" t="s">
+        <v>112</v>
+      </c>
+      <c r="C102">
+        <v>0.3</v>
+      </c>
+      <c r="D102" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A103" s="6">
+        <v>42858</v>
+      </c>
+      <c r="B103" t="s">
+        <v>113</v>
+      </c>
+      <c r="C103">
+        <v>0.5</v>
+      </c>
+      <c r="D103" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A104" s="6">
+        <v>42858</v>
+      </c>
+      <c r="B104" t="s">
+        <v>114</v>
+      </c>
+      <c r="C104">
+        <v>0.2</v>
+      </c>
+      <c r="D104" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A105" s="6">
+        <v>42861</v>
+      </c>
+      <c r="B105" t="s">
+        <v>115</v>
+      </c>
+      <c r="C105">
+        <v>0.5</v>
+      </c>
+      <c r="D105" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A106" s="6">
+        <v>42865</v>
+      </c>
+      <c r="B106" t="s">
+        <v>123</v>
+      </c>
+      <c r="C106">
+        <v>0.5</v>
+      </c>
+      <c r="D106" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A107" s="6">
+        <v>42865</v>
+      </c>
+      <c r="B107" t="s">
+        <v>124</v>
+      </c>
+      <c r="C107">
+        <v>2</v>
+      </c>
+      <c r="D107" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A108" s="6">
+        <v>42865</v>
+      </c>
+      <c r="B108" t="s">
+        <v>125</v>
+      </c>
+      <c r="C108">
+        <v>0.5</v>
+      </c>
+      <c r="D108" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A109" s="6"/>
+    </row>
+    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A110" s="6"/>
+    </row>
+    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A111" s="6"/>
+    </row>
+    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A112" s="6"/>
+    </row>
+    <row r="113" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A113" s="6"/>
+    </row>
+    <row r="114" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A114" s="6"/>
+      <c r="C114">
+        <f>SUM(C2:C113)</f>
+        <v>112.55000000000003</v>
+      </c>
+    </row>
+    <row r="115" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A115" s="6"/>
+    </row>
+    <row r="116" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A116" s="6"/>
+    </row>
+    <row r="117" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A117" s="6"/>
+    </row>
+    <row r="118" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A118" s="6"/>
+    </row>
+    <row r="119" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A119" s="6"/>
+    </row>
+    <row r="120" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A120" s="6"/>
+    </row>
+    <row r="121" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A121" s="6"/>
+    </row>
+    <row r="122" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A122" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>